<commit_message>
starting to add zips to tracts in disease data
</commit_message>
<xml_diff>
--- a/Data/CDC data/nashdisease2016.xlsx
+++ b/Data/CDC data/nashdisease2016.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k.simmons/Desktop/NSS/data analytics bootcamp/capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k.simmons/Desktop/NSS/data analytics bootcamp/capstone/Data/CDC data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D471BDB3-DBF6-5A48-A42F-68C6112AD3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01558E1-28A8-0E46-A628-D8D366D3EA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="47680" windowHeight="26420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12199,472 +12199,472 @@
     <t>(24.2, 42.5)</t>
   </si>
   <si>
-    <t>(36.1576629645, -86.8057331508)</t>
-  </si>
-  <si>
-    <t>(36.2758406196, -86.7227516725)</t>
-  </si>
-  <si>
-    <t>(36.0133154771, -86.7176062426)</t>
-  </si>
-  <si>
-    <t>(36.2962421445, -86.884373603)</t>
-  </si>
-  <si>
-    <t>(36.1231320505, -86.7142265091)</t>
-  </si>
-  <si>
-    <t>(36.1860223442, -86.7643746828)</t>
-  </si>
-  <si>
-    <t>(36.0304702133, -86.7544989419)</t>
-  </si>
-  <si>
-    <t>(36.2212110254, -86.7946381366)</t>
-  </si>
-  <si>
-    <t>(36.1342444257, -86.9660257669)</t>
-  </si>
-  <si>
-    <t>(36.2104122971, -86.6882030885)</t>
-  </si>
-  <si>
-    <t>(36.0851071347, -86.6579014347)</t>
-  </si>
-  <si>
-    <t>(36.1454955363, -86.7638145949)</t>
-  </si>
-  <si>
-    <t>(36.120319646, -86.7820995582)</t>
-  </si>
-  <si>
-    <t>(36.1286948607, -86.7851320823)</t>
-  </si>
-  <si>
-    <t>(36.2021376395, -86.7609246036)</t>
-  </si>
-  <si>
-    <t>(36.2156183387, -86.922992251)</t>
-  </si>
-  <si>
-    <t>(36.1215972147, -86.8291852595)</t>
-  </si>
-  <si>
-    <t>(36.0972128283, -86.5907016995)</t>
-  </si>
-  <si>
-    <t>(36.1006385723, -86.7268837685)</t>
-  </si>
-  <si>
-    <t>(36.2947153831, -86.6911187036)</t>
-  </si>
-  <si>
-    <t>(36.0886699253, -86.6809974727)</t>
-  </si>
-  <si>
-    <t>(36.0702023848, -86.6951799025)</t>
-  </si>
-  <si>
-    <t>(36.042374025, -86.7688478485)</t>
-  </si>
-  <si>
-    <t>(36.0627541445, -86.6647320159)</t>
-  </si>
-  <si>
-    <t>(36.1457801977, -86.8050873817)</t>
-  </si>
-  <si>
-    <t>(36.0931627912, -86.8736555705)</t>
-  </si>
-  <si>
-    <t>(36.2229163853, -86.7598911314)</t>
-  </si>
-  <si>
-    <t>(36.1711531762, -86.752019091)</t>
-  </si>
-  <si>
-    <t>(36.2059653483, -86.7961197587)</t>
-  </si>
-  <si>
-    <t>(36.1709368867, -86.644421803)</t>
-  </si>
-  <si>
-    <t>(36.0593607088, -86.7364092465)</t>
-  </si>
-  <si>
-    <t>(36.1714412594, -86.8285203739)</t>
-  </si>
-  <si>
-    <t>(36.2488660642, -86.8538782901)</t>
-  </si>
-  <si>
-    <t>(36.1911511856, -86.8085327041)</t>
-  </si>
-  <si>
-    <t>(36.1790862802, -86.7590618024)</t>
-  </si>
-  <si>
-    <t>(36.0521853395, -86.9407121165)</t>
-  </si>
-  <si>
-    <t>(35.9996029242, -86.6586366088)</t>
-  </si>
-  <si>
-    <t>(36.1804768223, -86.7383080372)</t>
-  </si>
-  <si>
-    <t>(36.1106881287, -86.8763668451)</t>
-  </si>
-  <si>
-    <t>(36.0657786763, -86.7267065082)</t>
-  </si>
-  <si>
-    <t>(36.2509916244, -86.731871255)</t>
-  </si>
-  <si>
-    <t>(36.1851740179, -86.6053672734)</t>
-  </si>
-  <si>
-    <t>(36.0995287373, -86.7996847381)</t>
-  </si>
-  <si>
-    <t>(36.1612468521, -86.8156490258)</t>
-  </si>
-  <si>
-    <t>(36.0532072157, -86.6572040786)</t>
-  </si>
-  <si>
-    <t>(36.344971962, -86.7677653742)</t>
-  </si>
-  <si>
-    <t>(36.0587984091, -86.6901293191)</t>
-  </si>
-  <si>
-    <t>(36.1439613559, -86.8662660609)</t>
-  </si>
-  <si>
-    <t>(36.2230900506, -86.6632138216)</t>
-  </si>
-  <si>
-    <t>(36.0848148306, -86.7119860954)</t>
-  </si>
-  <si>
-    <t>(36.0810876055, -86.6188609306)</t>
-  </si>
-  <si>
-    <t>(36.1133065622, -86.7274177563)</t>
-  </si>
-  <si>
-    <t>(36.1068258846, -86.7023156259)</t>
-  </si>
-  <si>
-    <t>(36.1728286331, -86.6903581821)</t>
-  </si>
-  <si>
-    <t>(36.2111454796, -86.7293550121)</t>
-  </si>
-  <si>
-    <t>(36.1836001359, -86.8846679987)</t>
-  </si>
-  <si>
-    <t>(36.0899457741, -86.7174801595)</t>
-  </si>
-  <si>
-    <t>(36.1125202586, -86.7940986863)</t>
-  </si>
-  <si>
-    <t>(36.0609096698, -86.8696928139)</t>
-  </si>
-  <si>
-    <t>(36.2287255904, -86.6339493996)</t>
-  </si>
-  <si>
-    <t>(36.1360963098, -86.7411039245)</t>
-  </si>
-  <si>
-    <t>(36.1446955813, -86.8426724912)</t>
-  </si>
-  <si>
-    <t>(36.175652119, -86.814804507)</t>
-  </si>
-  <si>
-    <t>(36.1597837914, -86.8530700515)</t>
-  </si>
-  <si>
-    <t>(36.0383226992, -86.6692426787)</t>
-  </si>
-  <si>
-    <t>(36.2343195911, -86.7732117462)</t>
-  </si>
-  <si>
-    <t>(36.0679630565, -86.8949107152)</t>
-  </si>
-  <si>
-    <t>(36.0506682578, -86.6371112264)</t>
-  </si>
-  <si>
-    <t>(36.1523856593, -86.6522822722)</t>
-  </si>
-  <si>
-    <t>(36.1457359079, -86.6254409227)</t>
-  </si>
-  <si>
-    <t>(36.1460702635, -86.8156944707)</t>
-  </si>
-  <si>
-    <t>(36.1719689182, -86.6206020339)</t>
-  </si>
-  <si>
-    <t>(36.1399427822, -86.7819906718)</t>
-  </si>
-  <si>
-    <t>(36.0971117892, -86.7878147099)</t>
-  </si>
-  <si>
-    <t>(36.1701688187, -86.7363924126)</t>
-  </si>
-  <si>
-    <t>(36.0873432616, -86.932612223)</t>
-  </si>
-  <si>
-    <t>(36.194381526, -86.6421905953)</t>
-  </si>
-  <si>
-    <t>(36.0192103596, -86.6464353266)</t>
-  </si>
-  <si>
-    <t>(36.1329172709, -86.8300431737)</t>
-  </si>
-  <si>
-    <t>(36.1839455221, -86.5833021676)</t>
-  </si>
-  <si>
-    <t>(36.1195178608, -86.7427999612)</t>
-  </si>
-  <si>
-    <t>(36.1346828403, -86.7023819538)</t>
-  </si>
-  <si>
-    <t>(36.1834698574, -86.7113792554)</t>
-  </si>
-  <si>
-    <t>(36.0753128653, -86.7434576848)</t>
-  </si>
-  <si>
-    <t>(36.0517956287, -86.7048611505)</t>
-  </si>
-  <si>
-    <t>(36.253365324, -86.6817557329)</t>
-  </si>
-  <si>
-    <t>(36.0460647087, -86.9719220455)</t>
-  </si>
-  <si>
-    <t>(36.2652149217, -86.7586096067)</t>
-  </si>
-  <si>
-    <t>(36.1562850243, -86.6793913918)</t>
-  </si>
-  <si>
-    <t>(36.0707379004, -86.8228348529)</t>
-  </si>
-  <si>
-    <t>(36.2882514084, -86.7728204615)</t>
-  </si>
-  <si>
-    <t>(36.1777432202, -86.790108485)</t>
-  </si>
-  <si>
-    <t>(36.1017022136, -86.6046378648)</t>
-  </si>
-  <si>
-    <t>(36.1276431581, -86.8678623837)</t>
-  </si>
-  <si>
-    <t>(36.2246054475, -86.7196053106)</t>
-  </si>
-  <si>
-    <t>(36.1503310917, -86.8286410961)</t>
-  </si>
-  <si>
-    <t>(36.069945042, -86.7140695527)</t>
-  </si>
-  <si>
-    <t>(36.1757150934, -86.8056204212)</t>
-  </si>
-  <si>
-    <t>(36.0513249553, -86.724258158)</t>
-  </si>
-  <si>
-    <t>(36.15764352, -86.7816792716)</t>
-  </si>
-  <si>
-    <t>(36.0300312489, -86.6145110967)</t>
-  </si>
-  <si>
-    <t>(36.1267253014, -86.634377235)</t>
-  </si>
-  <si>
-    <t>(36.0715952616, -86.9578354061)</t>
-  </si>
-  <si>
-    <t>(36.204125401, -86.7098381564)</t>
-  </si>
-  <si>
-    <t>(36.190570195, -86.855339398)</t>
-  </si>
-  <si>
-    <t>(36.1082517917, -86.8268057504)</t>
-  </si>
-  <si>
-    <t>(36.197632419, -86.6144973804)</t>
-  </si>
-  <si>
-    <t>(36.148106453, -86.5856887267)</t>
-  </si>
-  <si>
-    <t>(36.2729362225, -86.6610202749)</t>
-  </si>
-  <si>
-    <t>(36.1153457153, -86.8913814952)</t>
-  </si>
-  <si>
-    <t>(36.1431909387, -86.7899130999)</t>
-  </si>
-  <si>
-    <t>(36.1350470326, -86.8100174335)</t>
-  </si>
-  <si>
-    <t>(36.1582500552, -86.8715276437)</t>
-  </si>
-  <si>
-    <t>(36.073922218, -86.6732926633)</t>
-  </si>
-  <si>
-    <t>(36.1363692187, -86.7683698189)</t>
-  </si>
-  <si>
-    <t>(36.2269478533, -86.6077806723)</t>
-  </si>
-  <si>
-    <t>(36.049231748, -86.6797916232)</t>
-  </si>
-  <si>
-    <t>(36.2557501251, -86.7050849585)</t>
-  </si>
-  <si>
-    <t>(36.3479505187, -86.8675409005)</t>
-  </si>
-  <si>
-    <t>(36.0401325074, -87.0176548329)</t>
-  </si>
-  <si>
-    <t>(36.0842376102, -86.7415232924)</t>
-  </si>
-  <si>
-    <t>(36.2493399768, -86.7638027805)</t>
-  </si>
-  <si>
-    <t>(36.0696879457, -86.6150485034)</t>
-  </si>
-  <si>
-    <t>(36.124158094, -86.7550707151)</t>
-  </si>
-  <si>
-    <t>(36.1895940492, -86.7439426762)</t>
-  </si>
-  <si>
-    <t>(36.1353822457, -86.7150553656)</t>
-  </si>
-  <si>
-    <t>(36.151096554, -86.7597078621)</t>
-  </si>
-  <si>
-    <t>(36.1871201603, -86.7719899728)</t>
-  </si>
-  <si>
-    <t>(36.0320124181, -86.7277054628)</t>
-  </si>
-  <si>
-    <t>(36.0655938524, -86.9777719034)</t>
-  </si>
-  <si>
-    <t>(36.0524304194, -86.8041894006)</t>
-  </si>
-  <si>
-    <t>(36.0999620431, -86.639123776)</t>
-  </si>
-  <si>
-    <t>(36.0831866378, -86.5615305811)</t>
-  </si>
-  <si>
-    <t>(36.2059453952, -86.5921345588)</t>
-  </si>
-  <si>
-    <t>(36.1012139547, -86.7435789922)</t>
-  </si>
-  <si>
-    <t>(36.1247951937, -86.8014921222)</t>
-  </si>
-  <si>
-    <t>(36.0712760339, -86.9382627391)</t>
-  </si>
-  <si>
-    <t>(36.2249944111, -86.7399718241)</t>
-  </si>
-  <si>
-    <t>(36.1711444309, -86.768865228)</t>
-  </si>
-  <si>
-    <t>(36.1538311711, -86.7221674827)</t>
-  </si>
-  <si>
-    <t>(36.1514089398, -86.8836263472)</t>
-  </si>
-  <si>
-    <t>(36.166932328, -86.8036510368)</t>
-  </si>
-  <si>
-    <t>(36.0960612808, -86.8261504838)</t>
-  </si>
-  <si>
-    <t>(36.2681195238, -86.6959751266)</t>
-  </si>
-  <si>
-    <t>(36.1639335636, -86.8274060699)</t>
-  </si>
-  <si>
-    <t>(36.0722889795, -86.6476420172)</t>
-  </si>
-  <si>
-    <t>(36.0973117939, -86.908717199)</t>
-  </si>
-  <si>
-    <t>(36.1401682761, -86.7966089777)</t>
-  </si>
-  <si>
-    <t>(36.2537083567, -86.803607107)</t>
-  </si>
-  <si>
-    <t>(36.1985224304, -86.7337794886)</t>
-  </si>
-  <si>
-    <t>(36.0449466794, -86.7359377605)</t>
-  </si>
-  <si>
-    <t>(36.2080299864, -86.8352588264)</t>
-  </si>
-  <si>
-    <t>(36.0609917887, -86.7571314086)</t>
-  </si>
-  <si>
-    <t>(36.0769982456, -86.7054436498)</t>
-  </si>
-  <si>
-    <t>(36.0360852644, -86.6924294734)</t>
-  </si>
-  <si>
-    <t>(36.2432209865, -86.7170424941)</t>
+    <t>36.1576629645, -86.8057331508</t>
+  </si>
+  <si>
+    <t>36.2758406196, -86.7227516725</t>
+  </si>
+  <si>
+    <t>36.0133154771, -86.7176062426</t>
+  </si>
+  <si>
+    <t>36.2962421445, -86.884373603</t>
+  </si>
+  <si>
+    <t>36.1231320505, -86.7142265091</t>
+  </si>
+  <si>
+    <t>36.1860223442, -86.7643746828</t>
+  </si>
+  <si>
+    <t>36.0304702133, -86.7544989419</t>
+  </si>
+  <si>
+    <t>36.2212110254, -86.7946381366</t>
+  </si>
+  <si>
+    <t>36.1342444257, -86.9660257669</t>
+  </si>
+  <si>
+    <t>36.2104122971, -86.6882030885</t>
+  </si>
+  <si>
+    <t>36.0851071347, -86.6579014347</t>
+  </si>
+  <si>
+    <t>36.1454955363, -86.7638145949</t>
+  </si>
+  <si>
+    <t>36.120319646, -86.7820995582</t>
+  </si>
+  <si>
+    <t>36.1286948607, -86.7851320823</t>
+  </si>
+  <si>
+    <t>36.2021376395, -86.7609246036</t>
+  </si>
+  <si>
+    <t>36.2156183387, -86.922992251</t>
+  </si>
+  <si>
+    <t>36.1215972147, -86.8291852595</t>
+  </si>
+  <si>
+    <t>36.0972128283, -86.5907016995</t>
+  </si>
+  <si>
+    <t>36.1006385723, -86.7268837685</t>
+  </si>
+  <si>
+    <t>36.2947153831, -86.6911187036</t>
+  </si>
+  <si>
+    <t>36.0886699253, -86.6809974727</t>
+  </si>
+  <si>
+    <t>36.0702023848, -86.6951799025</t>
+  </si>
+  <si>
+    <t>36.042374025, -86.7688478485</t>
+  </si>
+  <si>
+    <t>36.0627541445, -86.6647320159</t>
+  </si>
+  <si>
+    <t>36.1457801977, -86.8050873817</t>
+  </si>
+  <si>
+    <t>36.0931627912, -86.8736555705</t>
+  </si>
+  <si>
+    <t>36.2229163853, -86.7598911314</t>
+  </si>
+  <si>
+    <t>36.1711531762, -86.752019091</t>
+  </si>
+  <si>
+    <t>36.2059653483, -86.7961197587</t>
+  </si>
+  <si>
+    <t>36.1709368867, -86.644421803</t>
+  </si>
+  <si>
+    <t>36.0593607088, -86.7364092465</t>
+  </si>
+  <si>
+    <t>36.1714412594, -86.8285203739</t>
+  </si>
+  <si>
+    <t>36.2488660642, -86.8538782901</t>
+  </si>
+  <si>
+    <t>36.1911511856, -86.8085327041</t>
+  </si>
+  <si>
+    <t>36.1790862802, -86.7590618024</t>
+  </si>
+  <si>
+    <t>36.0521853395, -86.9407121165</t>
+  </si>
+  <si>
+    <t>35.9996029242, -86.6586366088</t>
+  </si>
+  <si>
+    <t>36.1804768223, -86.7383080372</t>
+  </si>
+  <si>
+    <t>36.1106881287, -86.8763668451</t>
+  </si>
+  <si>
+    <t>36.0657786763, -86.7267065082</t>
+  </si>
+  <si>
+    <t>36.2509916244, -86.731871255</t>
+  </si>
+  <si>
+    <t>36.1851740179, -86.6053672734</t>
+  </si>
+  <si>
+    <t>36.0995287373, -86.7996847381</t>
+  </si>
+  <si>
+    <t>36.1612468521, -86.8156490258</t>
+  </si>
+  <si>
+    <t>36.0532072157, -86.6572040786</t>
+  </si>
+  <si>
+    <t>36.344971962, -86.7677653742</t>
+  </si>
+  <si>
+    <t>36.0587984091, -86.6901293191</t>
+  </si>
+  <si>
+    <t>36.1439613559, -86.8662660609</t>
+  </si>
+  <si>
+    <t>36.2230900506, -86.6632138216</t>
+  </si>
+  <si>
+    <t>36.0848148306, -86.7119860954</t>
+  </si>
+  <si>
+    <t>36.0810876055, -86.6188609306</t>
+  </si>
+  <si>
+    <t>36.1133065622, -86.7274177563</t>
+  </si>
+  <si>
+    <t>36.1068258846, -86.7023156259</t>
+  </si>
+  <si>
+    <t>36.1728286331, -86.6903581821</t>
+  </si>
+  <si>
+    <t>36.2111454796, -86.7293550121</t>
+  </si>
+  <si>
+    <t>36.1836001359, -86.8846679987</t>
+  </si>
+  <si>
+    <t>36.0899457741, -86.7174801595</t>
+  </si>
+  <si>
+    <t>36.1125202586, -86.7940986863</t>
+  </si>
+  <si>
+    <t>36.0609096698, -86.8696928139</t>
+  </si>
+  <si>
+    <t>36.2287255904, -86.6339493996</t>
+  </si>
+  <si>
+    <t>36.1360963098, -86.7411039245</t>
+  </si>
+  <si>
+    <t>36.1446955813, -86.8426724912</t>
+  </si>
+  <si>
+    <t>36.175652119, -86.814804507</t>
+  </si>
+  <si>
+    <t>36.1597837914, -86.8530700515</t>
+  </si>
+  <si>
+    <t>36.0383226992, -86.6692426787</t>
+  </si>
+  <si>
+    <t>36.2343195911, -86.7732117462</t>
+  </si>
+  <si>
+    <t>36.0679630565, -86.8949107152</t>
+  </si>
+  <si>
+    <t>36.0506682578, -86.6371112264</t>
+  </si>
+  <si>
+    <t>36.1523856593, -86.6522822722</t>
+  </si>
+  <si>
+    <t>36.1457359079, -86.6254409227</t>
+  </si>
+  <si>
+    <t>36.1460702635, -86.8156944707</t>
+  </si>
+  <si>
+    <t>36.1719689182, -86.6206020339</t>
+  </si>
+  <si>
+    <t>36.1399427822, -86.7819906718</t>
+  </si>
+  <si>
+    <t>36.0971117892, -86.7878147099</t>
+  </si>
+  <si>
+    <t>36.1701688187, -86.7363924126</t>
+  </si>
+  <si>
+    <t>36.0873432616, -86.932612223</t>
+  </si>
+  <si>
+    <t>36.194381526, -86.6421905953</t>
+  </si>
+  <si>
+    <t>36.0192103596, -86.6464353266</t>
+  </si>
+  <si>
+    <t>36.1329172709, -86.8300431737</t>
+  </si>
+  <si>
+    <t>36.1839455221, -86.5833021676</t>
+  </si>
+  <si>
+    <t>36.1195178608, -86.7427999612</t>
+  </si>
+  <si>
+    <t>36.1346828403, -86.7023819538</t>
+  </si>
+  <si>
+    <t>36.1834698574, -86.7113792554</t>
+  </si>
+  <si>
+    <t>36.0753128653, -86.7434576848</t>
+  </si>
+  <si>
+    <t>36.0517956287, -86.7048611505</t>
+  </si>
+  <si>
+    <t>36.253365324, -86.6817557329</t>
+  </si>
+  <si>
+    <t>36.0460647087, -86.9719220455</t>
+  </si>
+  <si>
+    <t>36.2652149217, -86.7586096067</t>
+  </si>
+  <si>
+    <t>36.1562850243, -86.6793913918</t>
+  </si>
+  <si>
+    <t>36.0707379004, -86.8228348529</t>
+  </si>
+  <si>
+    <t>36.2882514084, -86.7728204615</t>
+  </si>
+  <si>
+    <t>36.1777432202, -86.790108485</t>
+  </si>
+  <si>
+    <t>36.1017022136, -86.6046378648</t>
+  </si>
+  <si>
+    <t>36.1276431581, -86.8678623837</t>
+  </si>
+  <si>
+    <t>36.2246054475, -86.7196053106</t>
+  </si>
+  <si>
+    <t>36.1503310917, -86.8286410961</t>
+  </si>
+  <si>
+    <t>36.069945042, -86.7140695527</t>
+  </si>
+  <si>
+    <t>36.1757150934, -86.8056204212</t>
+  </si>
+  <si>
+    <t>36.0513249553, -86.724258158</t>
+  </si>
+  <si>
+    <t>36.15764352, -86.7816792716</t>
+  </si>
+  <si>
+    <t>36.0300312489, -86.6145110967</t>
+  </si>
+  <si>
+    <t>36.1267253014, -86.634377235</t>
+  </si>
+  <si>
+    <t>36.0715952616, -86.9578354061</t>
+  </si>
+  <si>
+    <t>36.204125401, -86.7098381564</t>
+  </si>
+  <si>
+    <t>36.190570195, -86.855339398</t>
+  </si>
+  <si>
+    <t>36.1082517917, -86.8268057504</t>
+  </si>
+  <si>
+    <t>36.197632419, -86.6144973804</t>
+  </si>
+  <si>
+    <t>36.148106453, -86.5856887267</t>
+  </si>
+  <si>
+    <t>36.2729362225, -86.6610202749</t>
+  </si>
+  <si>
+    <t>36.1153457153, -86.8913814952</t>
+  </si>
+  <si>
+    <t>36.1431909387, -86.7899130999</t>
+  </si>
+  <si>
+    <t>36.1350470326, -86.8100174335</t>
+  </si>
+  <si>
+    <t>36.1582500552, -86.8715276437</t>
+  </si>
+  <si>
+    <t>36.073922218, -86.6732926633</t>
+  </si>
+  <si>
+    <t>36.1363692187, -86.7683698189</t>
+  </si>
+  <si>
+    <t>36.2269478533, -86.6077806723</t>
+  </si>
+  <si>
+    <t>36.049231748, -86.6797916232</t>
+  </si>
+  <si>
+    <t>36.2557501251, -86.7050849585</t>
+  </si>
+  <si>
+    <t>36.3479505187, -86.8675409005</t>
+  </si>
+  <si>
+    <t>36.0401325074, -87.0176548329</t>
+  </si>
+  <si>
+    <t>36.0842376102, -86.7415232924</t>
+  </si>
+  <si>
+    <t>36.2493399768, -86.7638027805</t>
+  </si>
+  <si>
+    <t>36.0696879457, -86.6150485034</t>
+  </si>
+  <si>
+    <t>36.124158094, -86.7550707151</t>
+  </si>
+  <si>
+    <t>36.1895940492, -86.7439426762</t>
+  </si>
+  <si>
+    <t>36.1353822457, -86.7150553656</t>
+  </si>
+  <si>
+    <t>36.151096554, -86.7597078621</t>
+  </si>
+  <si>
+    <t>36.1871201603, -86.7719899728</t>
+  </si>
+  <si>
+    <t>36.0320124181, -86.7277054628</t>
+  </si>
+  <si>
+    <t>36.0655938524, -86.9777719034</t>
+  </si>
+  <si>
+    <t>36.0524304194, -86.8041894006</t>
+  </si>
+  <si>
+    <t>36.0999620431, -86.639123776</t>
+  </si>
+  <si>
+    <t>36.0831866378, -86.5615305811</t>
+  </si>
+  <si>
+    <t>36.2059453952, -86.5921345588</t>
+  </si>
+  <si>
+    <t>36.1012139547, -86.7435789922</t>
+  </si>
+  <si>
+    <t>36.1247951937, -86.8014921222</t>
+  </si>
+  <si>
+    <t>36.0712760339, -86.9382627391</t>
+  </si>
+  <si>
+    <t>36.2249944111, -86.7399718241</t>
+  </si>
+  <si>
+    <t>36.1711444309, -86.768865228</t>
+  </si>
+  <si>
+    <t>36.1538311711, -86.7221674827</t>
+  </si>
+  <si>
+    <t>36.1514089398, -86.8836263472</t>
+  </si>
+  <si>
+    <t>36.166932328, -86.8036510368</t>
+  </si>
+  <si>
+    <t>36.0960612808, -86.8261504838</t>
+  </si>
+  <si>
+    <t>36.2681195238, -86.6959751266</t>
+  </si>
+  <si>
+    <t>36.1639335636, -86.8274060699</t>
+  </si>
+  <si>
+    <t>36.0722889795, -86.6476420172</t>
+  </si>
+  <si>
+    <t>36.0973117939, -86.908717199</t>
+  </si>
+  <si>
+    <t>36.1401682761, -86.7966089777</t>
+  </si>
+  <si>
+    <t>36.2537083567, -86.803607107</t>
+  </si>
+  <si>
+    <t>36.1985224304, -86.7337794886</t>
+  </si>
+  <si>
+    <t>36.0449466794, -86.7359377605</t>
+  </si>
+  <si>
+    <t>36.2080299864, -86.8352588264</t>
+  </si>
+  <si>
+    <t>36.0609917887, -86.7571314086</t>
+  </si>
+  <si>
+    <t>36.0769982456, -86.7054436498</t>
+  </si>
+  <si>
+    <t>36.0360852644, -86.6924294734</t>
+  </si>
+  <si>
+    <t>36.2432209865, -86.7170424941</t>
   </si>
 </sst>
 </file>
@@ -13068,9 +13068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BG1" sqref="BG1:BG1048576"/>
+      <selection pane="bottomLeft" activeCell="BL1" sqref="BL1:BL1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>